<commit_message>
TRYING TO SEARCH THE RIGHT ANSWER
</commit_message>
<xml_diff>
--- a/GasDist/Examples/Лужский абразивный февр2019 (архив 10).xlsx
+++ b/GasDist/Examples/Лужский абразивный февр2019 (архив 10).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Рабочее Актив\Распределение формула\проверка 20190418\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\source\repos\avasaris\GasDistribution\GasDist\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4F4664-6C2C-4C76-B585-4A3FD47CA8DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12885" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="src" sheetId="4" r:id="rId1"/>
@@ -21,17 +22,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">src!$A$1:$BR$21</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="97">
   <si>
     <t>Потребитель</t>
   </si>
@@ -327,7 +333,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -630,7 +636,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -787,17 +793,32 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -807,12 +828,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -826,15 +841,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -847,22 +853,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный_src" xfId="3"/>
-    <cellStyle name="Обычный_Автотор" xfId="4"/>
-    <cellStyle name="Обычный_Лист1" xfId="1"/>
-    <cellStyle name="Обычный_Ручное распределение" xfId="2"/>
+    <cellStyle name="Обычный_src" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный_Автотор" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Обычный_Лист1" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Обычный_Ручное распределение" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -899,7 +908,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -964,7 +979,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1029,7 +1050,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1094,7 +1121,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4"/>
+        <xdr:cNvPr id="5" name="Рисунок 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1159,7 +1192,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Рисунок 6"/>
+        <xdr:cNvPr id="7" name="Рисунок 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1224,7 +1263,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Рисунок 7"/>
+        <xdr:cNvPr id="8" name="Рисунок 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1289,7 +1334,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Рисунок 8"/>
+        <xdr:cNvPr id="9" name="Рисунок 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1354,7 +1405,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Рисунок 9"/>
+        <xdr:cNvPr id="10" name="Рисунок 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1419,7 +1476,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Рисунок 10"/>
+        <xdr:cNvPr id="11" name="Рисунок 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1484,7 +1547,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Рисунок 11"/>
+        <xdr:cNvPr id="12" name="Рисунок 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1549,7 +1618,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Рисунок 12"/>
+        <xdr:cNvPr id="13" name="Рисунок 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1614,7 +1689,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Рисунок 13"/>
+        <xdr:cNvPr id="14" name="Рисунок 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1684,7 +1765,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1749,7 +1836,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1814,7 +1907,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1879,7 +1978,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4"/>
+        <xdr:cNvPr id="5" name="Рисунок 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1944,7 +2049,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Овальная выноска 6"/>
+        <xdr:cNvPr id="7" name="Овальная выноска 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2014,7 +2125,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2079,7 +2196,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2144,7 +2267,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2209,7 +2338,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4"/>
+        <xdr:cNvPr id="5" name="Рисунок 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2274,7 +2409,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Рисунок 6"/>
+        <xdr:cNvPr id="7" name="Рисунок 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2339,7 +2480,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Рисунок 7"/>
+        <xdr:cNvPr id="8" name="Рисунок 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2404,7 +2551,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Рисунок 8"/>
+        <xdr:cNvPr id="9" name="Рисунок 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2469,7 +2622,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Рисунок 9"/>
+        <xdr:cNvPr id="10" name="Рисунок 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2539,7 +2698,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Рисунок 5"/>
+        <xdr:cNvPr id="6" name="Рисунок 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2604,7 +2769,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Рисунок 6"/>
+        <xdr:cNvPr id="7" name="Рисунок 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2669,7 +2840,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Рисунок 7"/>
+        <xdr:cNvPr id="8" name="Рисунок 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2734,7 +2911,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Рисунок 8"/>
+        <xdr:cNvPr id="9" name="Рисунок 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2799,7 +2982,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Рисунок 9"/>
+        <xdr:cNvPr id="10" name="Рисунок 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2864,7 +3053,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Рисунок 10"/>
+        <xdr:cNvPr id="11" name="Рисунок 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2929,7 +3124,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Рисунок 11"/>
+        <xdr:cNvPr id="12" name="Рисунок 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2994,7 +3195,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Рисунок 12"/>
+        <xdr:cNvPr id="13" name="Рисунок 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3309,7 +3516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5760,11 +5967,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BF44"/>
   <sheetViews>
-    <sheetView topLeftCell="AA10" workbookViewId="0">
-      <selection activeCell="AJ32" sqref="AJ32"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5779,51 +5986,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="AA1" s="64" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="AA1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="64"/>
-      <c r="AC1" s="64"/>
-      <c r="AH1" s="65" t="s">
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AH1" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
-      <c r="AM1" s="65"/>
-      <c r="AN1" s="65"/>
-      <c r="AO1" s="65"/>
-      <c r="AP1" s="65"/>
-      <c r="AQ1" s="65"/>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+      <c r="AK1" s="67"/>
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="66"/>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -5890,10 +6097,10 @@
       <c r="AC4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AH4" s="66" t="s">
+      <c r="AH4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="AI4" s="66"/>
+      <c r="AI4" s="65"/>
       <c r="AJ4" s="21"/>
       <c r="AK4" s="21"/>
       <c r="AL4" s="21"/>
@@ -5902,10 +6109,10 @@
       <c r="AO4" s="21"/>
       <c r="AP4" s="21"/>
       <c r="AQ4" s="21"/>
-      <c r="AR4" s="66" t="s">
+      <c r="AR4" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="AS4" s="66"/>
+      <c r="AS4" s="65"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
@@ -6003,91 +6210,91 @@
       <c r="A8" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67" t="s">
+      <c r="C8" s="64"/>
+      <c r="D8" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67" t="s">
+      <c r="E8" s="64"/>
+      <c r="F8" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67" t="s">
+      <c r="G8" s="64"/>
+      <c r="H8" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67" t="s">
+      <c r="I8" s="64"/>
+      <c r="J8" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="67"/>
+      <c r="K8" s="64"/>
       <c r="L8" s="26"/>
-      <c r="M8" s="67" t="s">
+      <c r="M8" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67" t="s">
+      <c r="N8" s="64"/>
+      <c r="O8" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="67" t="s">
+      <c r="P8" s="64"/>
+      <c r="Q8" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="R8" s="67"/>
-      <c r="S8" s="67" t="s">
+      <c r="R8" s="64"/>
+      <c r="S8" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="T8" s="67"/>
-      <c r="U8" s="67" t="s">
+      <c r="T8" s="64"/>
+      <c r="U8" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="V8" s="67"/>
+      <c r="V8" s="64"/>
       <c r="AE8" s="16" t="s">
         <v>20</v>
       </c>
       <c r="AF8" s="15"/>
-      <c r="AH8" s="67" t="s">
+      <c r="AH8" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="AI8" s="67"/>
-      <c r="AJ8" s="67" t="s">
+      <c r="AI8" s="64"/>
+      <c r="AJ8" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="AK8" s="67"/>
-      <c r="AL8" s="67" t="s">
+      <c r="AK8" s="64"/>
+      <c r="AL8" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="AM8" s="67"/>
-      <c r="AN8" s="67" t="s">
+      <c r="AM8" s="64"/>
+      <c r="AN8" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="AO8" s="67"/>
-      <c r="AP8" s="67" t="s">
+      <c r="AO8" s="64"/>
+      <c r="AP8" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="AQ8" s="67"/>
-      <c r="AR8" s="67" t="s">
+      <c r="AQ8" s="64"/>
+      <c r="AR8" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="AS8" s="67"/>
-      <c r="AT8" s="67" t="s">
+      <c r="AS8" s="64"/>
+      <c r="AT8" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="AU8" s="67"/>
-      <c r="AV8" s="67" t="s">
+      <c r="AU8" s="64"/>
+      <c r="AV8" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="AW8" s="67"/>
-      <c r="AX8" s="67" t="s">
+      <c r="AW8" s="64"/>
+      <c r="AX8" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="AY8" s="67"/>
-      <c r="AZ8" s="67" t="s">
+      <c r="AY8" s="64"/>
+      <c r="AZ8" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="BA8" s="67"/>
+      <c r="BA8" s="64"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
@@ -6217,10 +6424,10 @@
         <f>AND(AB44&lt;B44,AC44&gt;0)</f>
         <v>0</v>
       </c>
-      <c r="AH11" s="66" t="s">
+      <c r="AH11" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="AI11" s="66"/>
+      <c r="AI11" s="65"/>
       <c r="AJ11" s="21"/>
       <c r="AK11" s="21"/>
       <c r="AL11" s="21"/>
@@ -6229,10 +6436,10 @@
       <c r="AO11" s="21"/>
       <c r="AP11" s="21"/>
       <c r="AQ11" s="21"/>
-      <c r="AR11" s="66" t="s">
+      <c r="AR11" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="AS11" s="66"/>
+      <c r="AS11" s="65"/>
       <c r="AT11" s="21"/>
       <c r="AU11" s="21"/>
       <c r="AV11" s="21"/>
@@ -7226,7 +7433,7 @@
         <v>0</v>
       </c>
       <c r="AZ20" s="27">
-        <f t="shared" si="15"/>
+        <f>V20-AP20</f>
         <v>1.371</v>
       </c>
       <c r="BA20" s="20">
@@ -10872,6 +11079,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AH1:AU1"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
     <mergeCell ref="AV8:AW8"/>
     <mergeCell ref="AX8:AY8"/>
     <mergeCell ref="AZ8:BA8"/>
@@ -10884,21 +11106,6 @@
     <mergeCell ref="AP8:AQ8"/>
     <mergeCell ref="AR8:AS8"/>
     <mergeCell ref="AT8:AU8"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AH1:AU1"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="AR4:AS4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10906,11 +11113,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BE48"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AL46" sqref="AL46"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10924,206 +11131,206 @@
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="70"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="75"/>
       <c r="AK1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" s="68" t="s">
+      <c r="AL1" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="69"/>
-      <c r="AO1" s="69"/>
-      <c r="AP1" s="69"/>
-      <c r="AQ1" s="69"/>
-      <c r="AR1" s="69"/>
-      <c r="AS1" s="69"/>
-      <c r="AT1" s="69"/>
-      <c r="AU1" s="69"/>
-      <c r="AV1" s="69"/>
-      <c r="AW1" s="69"/>
-      <c r="AX1" s="69"/>
-      <c r="AY1" s="69"/>
-      <c r="AZ1" s="69"/>
-      <c r="BA1" s="69"/>
-      <c r="BB1" s="69"/>
-      <c r="BC1" s="69"/>
-      <c r="BD1" s="69"/>
-      <c r="BE1" s="70"/>
+      <c r="AM1" s="74"/>
+      <c r="AN1" s="74"/>
+      <c r="AO1" s="74"/>
+      <c r="AP1" s="74"/>
+      <c r="AQ1" s="74"/>
+      <c r="AR1" s="74"/>
+      <c r="AS1" s="74"/>
+      <c r="AT1" s="74"/>
+      <c r="AU1" s="74"/>
+      <c r="AV1" s="74"/>
+      <c r="AW1" s="74"/>
+      <c r="AX1" s="74"/>
+      <c r="AY1" s="74"/>
+      <c r="AZ1" s="74"/>
+      <c r="BA1" s="74"/>
+      <c r="BB1" s="74"/>
+      <c r="BC1" s="74"/>
+      <c r="BD1" s="74"/>
+      <c r="BE1" s="75"/>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="68" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="70"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="75"/>
       <c r="AK2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="AL2" s="68" t="s">
+      <c r="AL2" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="AM2" s="69"/>
-      <c r="AN2" s="69"/>
-      <c r="AO2" s="69"/>
-      <c r="AP2" s="69"/>
-      <c r="AQ2" s="69"/>
-      <c r="AR2" s="69"/>
-      <c r="AS2" s="69"/>
-      <c r="AT2" s="69"/>
-      <c r="AU2" s="70"/>
-      <c r="AV2" s="68" t="s">
+      <c r="AM2" s="74"/>
+      <c r="AN2" s="74"/>
+      <c r="AO2" s="74"/>
+      <c r="AP2" s="74"/>
+      <c r="AQ2" s="74"/>
+      <c r="AR2" s="74"/>
+      <c r="AS2" s="74"/>
+      <c r="AT2" s="74"/>
+      <c r="AU2" s="75"/>
+      <c r="AV2" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="AW2" s="69"/>
-      <c r="AX2" s="69"/>
-      <c r="AY2" s="69"/>
-      <c r="AZ2" s="69"/>
-      <c r="BA2" s="69"/>
-      <c r="BB2" s="69"/>
-      <c r="BC2" s="69"/>
-      <c r="BD2" s="69"/>
-      <c r="BE2" s="70"/>
+      <c r="AW2" s="74"/>
+      <c r="AX2" s="74"/>
+      <c r="AY2" s="74"/>
+      <c r="AZ2" s="74"/>
+      <c r="BA2" s="74"/>
+      <c r="BB2" s="74"/>
+      <c r="BC2" s="74"/>
+      <c r="BD2" s="74"/>
+      <c r="BE2" s="75"/>
     </row>
     <row r="3" spans="1:57" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="70"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="75"/>
       <c r="AK3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="AM3" s="69"/>
-      <c r="AN3" s="69"/>
-      <c r="AO3" s="69"/>
-      <c r="AP3" s="69"/>
-      <c r="AQ3" s="69"/>
-      <c r="AR3" s="69"/>
-      <c r="AS3" s="69"/>
-      <c r="AT3" s="69"/>
-      <c r="AU3" s="69"/>
-      <c r="AV3" s="69"/>
-      <c r="AW3" s="69"/>
-      <c r="AX3" s="69"/>
-      <c r="AY3" s="69"/>
-      <c r="AZ3" s="69"/>
-      <c r="BA3" s="69"/>
-      <c r="BB3" s="69"/>
-      <c r="BC3" s="69"/>
-      <c r="BD3" s="69"/>
-      <c r="BE3" s="70"/>
+      <c r="AM3" s="74"/>
+      <c r="AN3" s="74"/>
+      <c r="AO3" s="74"/>
+      <c r="AP3" s="74"/>
+      <c r="AQ3" s="74"/>
+      <c r="AR3" s="74"/>
+      <c r="AS3" s="74"/>
+      <c r="AT3" s="74"/>
+      <c r="AU3" s="74"/>
+      <c r="AV3" s="74"/>
+      <c r="AW3" s="74"/>
+      <c r="AX3" s="74"/>
+      <c r="AY3" s="74"/>
+      <c r="AZ3" s="74"/>
+      <c r="BA3" s="74"/>
+      <c r="BB3" s="74"/>
+      <c r="BC3" s="74"/>
+      <c r="BD3" s="74"/>
+      <c r="BE3" s="75"/>
     </row>
     <row r="4" spans="1:57" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="71" t="s">
+      <c r="C4" s="69"/>
+      <c r="D4" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="71" t="s">
+      <c r="E4" s="69"/>
+      <c r="F4" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="72"/>
-      <c r="H4" s="71" t="s">
+      <c r="G4" s="69"/>
+      <c r="H4" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="71" t="s">
+      <c r="I4" s="69"/>
+      <c r="J4" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="72"/>
-      <c r="L4" s="71" t="s">
+      <c r="K4" s="69"/>
+      <c r="L4" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="72"/>
-      <c r="N4" s="71" t="s">
+      <c r="M4" s="69"/>
+      <c r="N4" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="72"/>
-      <c r="P4" s="71" t="s">
+      <c r="O4" s="69"/>
+      <c r="P4" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="71" t="s">
+      <c r="Q4" s="69"/>
+      <c r="R4" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="72"/>
-      <c r="T4" s="71" t="s">
+      <c r="S4" s="69"/>
+      <c r="T4" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="U4" s="72"/>
+      <c r="U4" s="69"/>
       <c r="W4" s="46" t="s">
         <v>31</v>
       </c>
@@ -11142,46 +11349,46 @@
       <c r="AK4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AL4" s="71" t="s">
+      <c r="AL4" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="AM4" s="72"/>
-      <c r="AN4" s="71" t="s">
+      <c r="AM4" s="69"/>
+      <c r="AN4" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="71" t="s">
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="71" t="s">
+      <c r="AQ4" s="69"/>
+      <c r="AR4" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="AS4" s="72"/>
-      <c r="AT4" s="71" t="s">
+      <c r="AS4" s="69"/>
+      <c r="AT4" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AU4" s="72"/>
-      <c r="AV4" s="71" t="s">
+      <c r="AU4" s="69"/>
+      <c r="AV4" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="AW4" s="72"/>
-      <c r="AX4" s="71" t="s">
+      <c r="AW4" s="69"/>
+      <c r="AX4" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="AY4" s="72"/>
-      <c r="AZ4" s="71" t="s">
+      <c r="AY4" s="69"/>
+      <c r="AZ4" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="BA4" s="72"/>
-      <c r="BB4" s="71" t="s">
+      <c r="BA4" s="69"/>
+      <c r="BB4" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="BC4" s="72"/>
-      <c r="BD4" s="71" t="s">
+      <c r="BC4" s="69"/>
+      <c r="BD4" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="BE4" s="72"/>
+      <c r="BE4" s="69"/>
     </row>
     <row r="5" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
@@ -11336,117 +11543,117 @@
       <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B6" s="76">
         <v>1</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="73">
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="76">
         <v>2</v>
       </c>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="74"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="75"/>
-      <c r="AG6" s="76" t="s">
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="77"/>
+      <c r="R6" s="77"/>
+      <c r="S6" s="77"/>
+      <c r="T6" s="77"/>
+      <c r="U6" s="78"/>
+      <c r="AG6" s="79" t="s">
         <v>17</v>
       </c>
       <c r="AK6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="AL6" s="73">
+      <c r="AL6" s="76">
         <v>1</v>
       </c>
-      <c r="AM6" s="74"/>
-      <c r="AN6" s="74"/>
-      <c r="AO6" s="74"/>
-      <c r="AP6" s="74"/>
-      <c r="AQ6" s="74"/>
-      <c r="AR6" s="74"/>
-      <c r="AS6" s="74"/>
-      <c r="AT6" s="74"/>
-      <c r="AU6" s="75"/>
-      <c r="AV6" s="73">
+      <c r="AM6" s="77"/>
+      <c r="AN6" s="77"/>
+      <c r="AO6" s="77"/>
+      <c r="AP6" s="77"/>
+      <c r="AQ6" s="77"/>
+      <c r="AR6" s="77"/>
+      <c r="AS6" s="77"/>
+      <c r="AT6" s="77"/>
+      <c r="AU6" s="78"/>
+      <c r="AV6" s="76">
         <v>2</v>
       </c>
-      <c r="AW6" s="74"/>
-      <c r="AX6" s="74"/>
-      <c r="AY6" s="74"/>
-      <c r="AZ6" s="74"/>
-      <c r="BA6" s="74"/>
-      <c r="BB6" s="74"/>
-      <c r="BC6" s="74"/>
-      <c r="BD6" s="74"/>
-      <c r="BE6" s="75"/>
+      <c r="AW6" s="77"/>
+      <c r="AX6" s="77"/>
+      <c r="AY6" s="77"/>
+      <c r="AZ6" s="77"/>
+      <c r="BA6" s="77"/>
+      <c r="BB6" s="77"/>
+      <c r="BC6" s="77"/>
+      <c r="BD6" s="77"/>
+      <c r="BE6" s="78"/>
     </row>
     <row r="7" spans="1:57" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="73">
+      <c r="B7" s="76">
         <v>1</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="73">
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="76">
         <v>2</v>
       </c>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="75"/>
-      <c r="AG7" s="76"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
+      <c r="R7" s="77"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="77"/>
+      <c r="U7" s="78"/>
+      <c r="AG7" s="79"/>
       <c r="AK7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AL7" s="73">
+      <c r="AL7" s="76">
         <v>1</v>
       </c>
-      <c r="AM7" s="74"/>
-      <c r="AN7" s="74"/>
-      <c r="AO7" s="74"/>
-      <c r="AP7" s="74"/>
-      <c r="AQ7" s="74"/>
-      <c r="AR7" s="74"/>
-      <c r="AS7" s="74"/>
-      <c r="AT7" s="74"/>
-      <c r="AU7" s="75"/>
-      <c r="AV7" s="73">
+      <c r="AM7" s="77"/>
+      <c r="AN7" s="77"/>
+      <c r="AO7" s="77"/>
+      <c r="AP7" s="77"/>
+      <c r="AQ7" s="77"/>
+      <c r="AR7" s="77"/>
+      <c r="AS7" s="77"/>
+      <c r="AT7" s="77"/>
+      <c r="AU7" s="78"/>
+      <c r="AV7" s="76">
         <v>2</v>
       </c>
-      <c r="AW7" s="74"/>
-      <c r="AX7" s="74"/>
-      <c r="AY7" s="74"/>
-      <c r="AZ7" s="74"/>
-      <c r="BA7" s="74"/>
-      <c r="BB7" s="74"/>
-      <c r="BC7" s="74"/>
-      <c r="BD7" s="74"/>
-      <c r="BE7" s="75"/>
+      <c r="AW7" s="77"/>
+      <c r="AX7" s="77"/>
+      <c r="AY7" s="77"/>
+      <c r="AZ7" s="77"/>
+      <c r="BA7" s="77"/>
+      <c r="BB7" s="77"/>
+      <c r="BC7" s="77"/>
+      <c r="BD7" s="77"/>
+      <c r="BE7" s="78"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
@@ -11748,11 +11955,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U10" s="41"/>
-      <c r="AC10" s="77" t="s">
+      <c r="AC10" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="AD10" s="78"/>
-      <c r="AE10" s="79"/>
+      <c r="AD10" s="71"/>
+      <c r="AE10" s="72"/>
       <c r="AK10" s="38" t="s">
         <v>10</v>
       </c>
@@ -11956,8 +12163,8 @@
       </c>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
-        <v>50</v>
+      <c r="A12" s="87">
+        <v>43497</v>
       </c>
       <c r="B12" s="44">
         <v>13.877000000000001</v>
@@ -12138,8 +12345,8 @@
       </c>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
-        <v>51</v>
+      <c r="A13" s="87">
+        <v>43498</v>
       </c>
       <c r="B13" s="44">
         <v>11.877000000000001</v>
@@ -12320,8 +12527,8 @@
       </c>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
-        <v>52</v>
+      <c r="A14" s="87">
+        <v>43499</v>
       </c>
       <c r="B14" s="44">
         <v>12.694000000000001</v>
@@ -12502,8 +12709,8 @@
       </c>
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
-        <v>53</v>
+      <c r="A15" s="87">
+        <v>43500</v>
       </c>
       <c r="B15" s="45">
         <v>10.75</v>
@@ -12684,8 +12891,8 @@
       </c>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
-        <v>54</v>
+      <c r="A16" s="87">
+        <v>43501</v>
       </c>
       <c r="B16" s="44">
         <v>11.566000000000001</v>
@@ -12866,8 +13073,8 @@
       </c>
     </row>
     <row r="17" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="s">
-        <v>55</v>
+      <c r="A17" s="87">
+        <v>43502</v>
       </c>
       <c r="B17" s="44">
         <v>12.801</v>
@@ -13048,8 +13255,8 @@
       </c>
     </row>
     <row r="18" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
-        <v>56</v>
+      <c r="A18" s="87">
+        <v>43503</v>
       </c>
       <c r="B18" s="44">
         <v>14.286</v>
@@ -13230,8 +13437,8 @@
       </c>
     </row>
     <row r="19" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
-        <v>57</v>
+      <c r="A19" s="87">
+        <v>43504</v>
       </c>
       <c r="B19" s="44">
         <v>12.967000000000001</v>
@@ -13412,8 +13619,8 @@
       </c>
     </row>
     <row r="20" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
-        <v>58</v>
+      <c r="A20" s="87">
+        <v>43505</v>
       </c>
       <c r="B20" s="44">
         <v>12.805</v>
@@ -13594,8 +13801,8 @@
       </c>
     </row>
     <row r="21" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
-        <v>59</v>
+      <c r="A21" s="87">
+        <v>43506</v>
       </c>
       <c r="B21" s="44">
         <v>11.733000000000001</v>
@@ -13776,8 +13983,8 @@
       </c>
     </row>
     <row r="22" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
-        <v>60</v>
+      <c r="A22" s="87">
+        <v>43507</v>
       </c>
       <c r="B22" s="44">
         <v>10.084</v>
@@ -13958,8 +14165,8 @@
       </c>
     </row>
     <row r="23" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A23" s="43" t="s">
-        <v>61</v>
+      <c r="A23" s="87">
+        <v>43508</v>
       </c>
       <c r="B23" s="44">
         <v>11.746</v>
@@ -14140,8 +14347,8 @@
       </c>
     </row>
     <row r="24" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A24" s="43" t="s">
-        <v>62</v>
+      <c r="A24" s="87">
+        <v>43509</v>
       </c>
       <c r="B24" s="44">
         <v>13.151999999999999</v>
@@ -14322,8 +14529,8 @@
       </c>
     </row>
     <row r="25" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
-        <v>63</v>
+      <c r="A25" s="87">
+        <v>43510</v>
       </c>
       <c r="B25" s="44">
         <v>12.568</v>
@@ -14504,8 +14711,8 @@
       </c>
     </row>
     <row r="26" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A26" s="43" t="s">
-        <v>64</v>
+      <c r="A26" s="87">
+        <v>43511</v>
       </c>
       <c r="B26" s="45">
         <v>11.63</v>
@@ -14686,8 +14893,8 @@
       </c>
     </row>
     <row r="27" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A27" s="43" t="s">
-        <v>65</v>
+      <c r="A27" s="87">
+        <v>43512</v>
       </c>
       <c r="B27" s="44">
         <v>12.670999999999999</v>
@@ -14868,8 +15075,8 @@
       </c>
     </row>
     <row r="28" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A28" s="43" t="s">
-        <v>66</v>
+      <c r="A28" s="87">
+        <v>43513</v>
       </c>
       <c r="B28" s="45">
         <v>12.96</v>
@@ -15050,8 +15257,8 @@
       </c>
     </row>
     <row r="29" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A29" s="43" t="s">
-        <v>67</v>
+      <c r="A29" s="87">
+        <v>43514</v>
       </c>
       <c r="B29" s="45">
         <v>13.37</v>
@@ -15232,8 +15439,8 @@
       </c>
     </row>
     <row r="30" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A30" s="43" t="s">
-        <v>68</v>
+      <c r="A30" s="87">
+        <v>43515</v>
       </c>
       <c r="B30" s="44">
         <v>14.286</v>
@@ -15414,8 +15621,8 @@
       </c>
     </row>
     <row r="31" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A31" s="43" t="s">
-        <v>69</v>
+      <c r="A31" s="87">
+        <v>43516</v>
       </c>
       <c r="B31" s="44">
         <v>12.457000000000001</v>
@@ -15596,8 +15803,8 @@
       </c>
     </row>
     <row r="32" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A32" s="43" t="s">
-        <v>70</v>
+      <c r="A32" s="87">
+        <v>43517</v>
       </c>
       <c r="B32" s="44">
         <v>14.286</v>
@@ -15778,8 +15985,8 @@
       </c>
     </row>
     <row r="33" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A33" s="43" t="s">
-        <v>71</v>
+      <c r="A33" s="87">
+        <v>43518</v>
       </c>
       <c r="B33" s="44">
         <v>14.285</v>
@@ -15960,8 +16167,8 @@
       </c>
     </row>
     <row r="34" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A34" s="43" t="s">
-        <v>72</v>
+      <c r="A34" s="87">
+        <v>43519</v>
       </c>
       <c r="B34" s="44">
         <v>12.872999999999999</v>
@@ -16142,8 +16349,8 @@
       </c>
     </row>
     <row r="35" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A35" s="43" t="s">
-        <v>73</v>
+      <c r="A35" s="87">
+        <v>43520</v>
       </c>
       <c r="B35" s="44">
         <v>10.452</v>
@@ -16324,8 +16531,8 @@
       </c>
     </row>
     <row r="36" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A36" s="43" t="s">
-        <v>74</v>
+      <c r="A36" s="87">
+        <v>43521</v>
       </c>
       <c r="B36" s="44">
         <v>12.391999999999999</v>
@@ -16506,8 +16713,8 @@
       </c>
     </row>
     <row r="37" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A37" s="43" t="s">
-        <v>75</v>
+      <c r="A37" s="87">
+        <v>43522</v>
       </c>
       <c r="B37" s="44">
         <v>12.083</v>
@@ -16688,8 +16895,8 @@
       </c>
     </row>
     <row r="38" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A38" s="43" t="s">
-        <v>76</v>
+      <c r="A38" s="87">
+        <v>43523</v>
       </c>
       <c r="B38" s="44">
         <v>10.832000000000001</v>
@@ -16870,8 +17077,8 @@
       </c>
     </row>
     <row r="39" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A39" s="43" t="s">
-        <v>77</v>
+      <c r="A39" s="87">
+        <v>43524</v>
       </c>
       <c r="B39" s="44">
         <v>10.692</v>
@@ -17292,6 +17499,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="B3:U3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AT4:AU4"/>
+    <mergeCell ref="AV4:AW4"/>
+    <mergeCell ref="AX4:AY4"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="L6:U6"/>
+    <mergeCell ref="L7:U7"/>
+    <mergeCell ref="AG6:AG7"/>
     <mergeCell ref="AZ4:BA4"/>
     <mergeCell ref="BB4:BC4"/>
     <mergeCell ref="BD4:BE4"/>
@@ -17308,28 +17537,6 @@
     <mergeCell ref="AV6:BE6"/>
     <mergeCell ref="AL7:AU7"/>
     <mergeCell ref="AV7:BE7"/>
-    <mergeCell ref="AT4:AU4"/>
-    <mergeCell ref="AV4:AW4"/>
-    <mergeCell ref="AX4:AY4"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="L6:U6"/>
-    <mergeCell ref="L7:U7"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="B1:U1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="L2:U2"/>
-    <mergeCell ref="B3:U3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17338,11 +17545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BO40"/>
   <sheetViews>
-    <sheetView topLeftCell="AM1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BE12" sqref="BE12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BO25" sqref="BO25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -17356,219 +17563,219 @@
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="70"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="74"/>
+      <c r="AC1" s="74"/>
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="75"/>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="68" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69"/>
-      <c r="AE2" s="70"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="74"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="74"/>
+      <c r="AC2" s="74"/>
+      <c r="AD2" s="74"/>
+      <c r="AE2" s="75"/>
     </row>
     <row r="3" spans="1:67" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="69"/>
-      <c r="V3" s="69"/>
-      <c r="W3" s="69"/>
-      <c r="X3" s="69"/>
-      <c r="Y3" s="69"/>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="69"/>
-      <c r="AB3" s="69"/>
-      <c r="AC3" s="69"/>
-      <c r="AD3" s="69"/>
-      <c r="AE3" s="70"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
+      <c r="Y3" s="74"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="74"/>
+      <c r="AC3" s="74"/>
+      <c r="AD3" s="74"/>
+      <c r="AE3" s="75"/>
     </row>
     <row r="4" spans="1:67" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="68" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="80"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="71" t="s">
+      <c r="D4" s="69"/>
+      <c r="E4" s="68" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="80"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="71" t="s">
+      <c r="G4" s="69"/>
+      <c r="H4" s="68" t="s">
         <v>33</v>
       </c>
       <c r="I4" s="80"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="71" t="s">
+      <c r="J4" s="69"/>
+      <c r="K4" s="68" t="s">
         <v>34</v>
       </c>
       <c r="L4" s="80"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="71" t="s">
+      <c r="M4" s="69"/>
+      <c r="N4" s="68" t="s">
         <v>35</v>
       </c>
       <c r="O4" s="80"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="71" t="s">
+      <c r="P4" s="69"/>
+      <c r="Q4" s="68" t="s">
         <v>31</v>
       </c>
       <c r="R4" s="80"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="71" t="s">
+      <c r="S4" s="69"/>
+      <c r="T4" s="68" t="s">
         <v>32</v>
       </c>
       <c r="U4" s="80"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="71" t="s">
+      <c r="V4" s="69"/>
+      <c r="W4" s="68" t="s">
         <v>33</v>
       </c>
       <c r="X4" s="80"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="71" t="s">
+      <c r="Y4" s="69"/>
+      <c r="Z4" s="68" t="s">
         <v>34</v>
       </c>
       <c r="AA4" s="80"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="71" t="s">
+      <c r="AB4" s="69"/>
+      <c r="AC4" s="68" t="s">
         <v>35</v>
       </c>
       <c r="AD4" s="80"/>
-      <c r="AE4" s="72"/>
-      <c r="AG4" s="71" t="s">
+      <c r="AE4" s="69"/>
+      <c r="AG4" s="68" t="s">
         <v>31</v>
       </c>
       <c r="AH4" s="80"/>
-      <c r="AI4" s="72"/>
-      <c r="AJ4" s="71" t="s">
+      <c r="AI4" s="69"/>
+      <c r="AJ4" s="68" t="s">
         <v>32</v>
       </c>
       <c r="AK4" s="80"/>
-      <c r="AL4" s="72"/>
-      <c r="AM4" s="71" t="s">
+      <c r="AL4" s="69"/>
+      <c r="AM4" s="68" t="s">
         <v>33</v>
       </c>
       <c r="AN4" s="80"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="71" t="s">
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="68" t="s">
         <v>34</v>
       </c>
       <c r="AQ4" s="80"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="71" t="s">
+      <c r="AR4" s="69"/>
+      <c r="AS4" s="68" t="s">
         <v>35</v>
       </c>
       <c r="AT4" s="80"/>
-      <c r="AU4" s="72"/>
-      <c r="BA4" s="71" t="s">
+      <c r="AU4" s="69"/>
+      <c r="BA4" s="68" t="s">
         <v>31</v>
       </c>
       <c r="BB4" s="80"/>
-      <c r="BC4" s="72"/>
-      <c r="BD4" s="71" t="s">
+      <c r="BC4" s="69"/>
+      <c r="BD4" s="68" t="s">
         <v>32</v>
       </c>
       <c r="BE4" s="80"/>
-      <c r="BF4" s="72"/>
-      <c r="BG4" s="71" t="s">
+      <c r="BF4" s="69"/>
+      <c r="BG4" s="68" t="s">
         <v>33</v>
       </c>
       <c r="BH4" s="80"/>
-      <c r="BI4" s="72"/>
-      <c r="BJ4" s="71" t="s">
+      <c r="BI4" s="69"/>
+      <c r="BJ4" s="68" t="s">
         <v>34</v>
       </c>
       <c r="BK4" s="80"/>
-      <c r="BL4" s="72"/>
-      <c r="BM4" s="71" t="s">
+      <c r="BL4" s="69"/>
+      <c r="BM4" s="68" t="s">
         <v>35</v>
       </c>
       <c r="BN4" s="80"/>
-      <c r="BO4" s="72"/>
+      <c r="BO4" s="69"/>
     </row>
     <row r="5" spans="1:67" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
@@ -17759,79 +17966,79 @@
       <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B6" s="76">
         <v>1</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="73">
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="76">
         <v>2</v>
       </c>
-      <c r="R6" s="74"/>
-      <c r="S6" s="74"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="74"/>
-      <c r="V6" s="74"/>
-      <c r="W6" s="74"/>
-      <c r="X6" s="74"/>
-      <c r="Y6" s="74"/>
-      <c r="Z6" s="74"/>
-      <c r="AA6" s="74"/>
-      <c r="AB6" s="74"/>
-      <c r="AC6" s="74"/>
-      <c r="AD6" s="74"/>
-      <c r="AE6" s="75"/>
+      <c r="R6" s="77"/>
+      <c r="S6" s="77"/>
+      <c r="T6" s="77"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="77"/>
+      <c r="W6" s="77"/>
+      <c r="X6" s="77"/>
+      <c r="Y6" s="77"/>
+      <c r="Z6" s="77"/>
+      <c r="AA6" s="77"/>
+      <c r="AB6" s="77"/>
+      <c r="AC6" s="77"/>
+      <c r="AD6" s="77"/>
+      <c r="AE6" s="78"/>
     </row>
     <row r="7" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="73">
+      <c r="B7" s="76">
         <v>1</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="73">
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="78"/>
+      <c r="Q7" s="76">
         <v>2</v>
       </c>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="74"/>
-      <c r="W7" s="74"/>
-      <c r="X7" s="74"/>
-      <c r="Y7" s="74"/>
-      <c r="Z7" s="74"/>
-      <c r="AA7" s="74"/>
-      <c r="AB7" s="74"/>
-      <c r="AC7" s="74"/>
-      <c r="AD7" s="74"/>
-      <c r="AE7" s="75"/>
+      <c r="R7" s="77"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="77"/>
+      <c r="U7" s="77"/>
+      <c r="V7" s="77"/>
+      <c r="W7" s="77"/>
+      <c r="X7" s="77"/>
+      <c r="Y7" s="77"/>
+      <c r="Z7" s="77"/>
+      <c r="AA7" s="77"/>
+      <c r="AB7" s="77"/>
+      <c r="AC7" s="77"/>
+      <c r="AD7" s="77"/>
+      <c r="AE7" s="78"/>
     </row>
     <row r="8" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
@@ -18119,11 +18326,11 @@
       <c r="AS10" s="82"/>
       <c r="AT10" s="82"/>
       <c r="AU10" s="83"/>
-      <c r="AW10" s="77" t="s">
+      <c r="AW10" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="AX10" s="78"/>
-      <c r="AY10" s="79"/>
+      <c r="AX10" s="71"/>
+      <c r="AY10" s="72"/>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
@@ -25151,6 +25358,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AG10:AU10"/>
+    <mergeCell ref="BG4:BI4"/>
+    <mergeCell ref="BJ4:BL4"/>
+    <mergeCell ref="BM4:BO4"/>
+    <mergeCell ref="AW10:AY10"/>
+    <mergeCell ref="AS4:AU4"/>
+    <mergeCell ref="BD4:BF4"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="Q6:AE6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="Q7:AE7"/>
+    <mergeCell ref="BA4:BC4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AM4:AO4"/>
+    <mergeCell ref="AJ4:AL4"/>
+    <mergeCell ref="AG4:AI4"/>
     <mergeCell ref="B1:AE1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="Q2:AE2"/>
@@ -25163,24 +25388,6 @@
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="Q6:AE6"/>
-    <mergeCell ref="B7:P7"/>
-    <mergeCell ref="Q7:AE7"/>
-    <mergeCell ref="BA4:BC4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AM4:AO4"/>
-    <mergeCell ref="AJ4:AL4"/>
-    <mergeCell ref="AG4:AI4"/>
-    <mergeCell ref="AG10:AU10"/>
-    <mergeCell ref="BG4:BI4"/>
-    <mergeCell ref="BJ4:BL4"/>
-    <mergeCell ref="BM4:BO4"/>
-    <mergeCell ref="AW10:AY10"/>
-    <mergeCell ref="AS4:AU4"/>
-    <mergeCell ref="BD4:BF4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25189,11 +25396,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AI52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC43" sqref="AC43:AF43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -25209,109 +25416,109 @@
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="86"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="84"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="68" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="86"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="84"/>
     </row>
     <row r="3" spans="1:35" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="86"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="84"/>
     </row>
     <row r="4" spans="1:35" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="68" t="s">
         <v>89</v>
       </c>
       <c r="C4" s="80"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="71" t="s">
+      <c r="D4" s="69"/>
+      <c r="E4" s="68" t="s">
         <v>90</v>
       </c>
       <c r="F4" s="80"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="71" t="str">
+      <c r="G4" s="69"/>
+      <c r="H4" s="68" t="str">
         <f>B4</f>
         <v>г. Калининград, Магнитогорская ул., д.4</v>
       </c>
       <c r="I4" s="80"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="71" t="str">
+      <c r="J4" s="69"/>
+      <c r="K4" s="68" t="str">
         <f>E4</f>
         <v>г. Калининград, Большая Окружная 4-я ул., д.1 А, котельная</v>
       </c>
       <c r="L4" s="80"/>
-      <c r="M4" s="72"/>
-      <c r="O4" s="71" t="str">
+      <c r="M4" s="69"/>
+      <c r="O4" s="68" t="str">
         <f>B4</f>
         <v>г. Калининград, Магнитогорская ул., д.4</v>
       </c>
       <c r="P4" s="80"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="71" t="str">
+      <c r="Q4" s="69"/>
+      <c r="R4" s="68" t="str">
         <f>E4</f>
         <v>г. Калининград, Большая Окружная 4-я ул., д.1 А, котельная</v>
       </c>
       <c r="S4" s="80"/>
-      <c r="T4" s="72"/>
-      <c r="V4" s="71" t="str">
+      <c r="T4" s="69"/>
+      <c r="V4" s="68" t="str">
         <f>B4</f>
         <v>г. Калининград, Магнитогорская ул., д.4</v>
       </c>
       <c r="W4" s="80"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="71" t="str">
+      <c r="X4" s="69"/>
+      <c r="Y4" s="68" t="str">
         <f>E4</f>
         <v>г. Калининград, Большая Окружная 4-я ул., д.1 А, котельная</v>
       </c>
       <c r="Z4" s="80"/>
-      <c r="AA4" s="72"/>
+      <c r="AA4" s="69"/>
       <c r="AC4" s="62" t="str">
         <f>V4</f>
         <v>г. Калининград, Магнитогорская ул., д.4</v>
@@ -25428,47 +25635,47 @@
       <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B6" s="76">
         <v>4</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="73">
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="76">
         <v>3</v>
       </c>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="85"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="86"/>
     </row>
     <row r="7" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="73">
+      <c r="B7" s="76">
         <v>3</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="73">
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="76">
         <v>4</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="85"/>
-      <c r="AD7" s="84" t="s">
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="86"/>
+      <c r="AD7" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="AE7" s="84"/>
+      <c r="AE7" s="85"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
@@ -25872,7 +26079,7 @@
         <v>2.3</v>
       </c>
       <c r="W13" s="3">
-        <f t="shared" ref="W12:W20" si="11">MIN(Q13,B13)</f>
+        <f t="shared" ref="W13:W20" si="11">MIN(Q13,B13)</f>
         <v>5.3230000000000004</v>
       </c>
       <c r="X13" s="3">
@@ -29490,6 +29697,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O10:T10"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:M2"/>
@@ -29497,17 +29715,6 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="H4:J4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="O10:T10"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Some research in examples
</commit_message>
<xml_diff>
--- a/GasDist/Examples/Лужский абразивный февр2019 (архив 10).xlsx
+++ b/GasDist/Examples/Лужский абразивный февр2019 (архив 10).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\source\repos\avasaris\GasDistribution\GasDist\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code PET\repos\GasDistribution\GasDist\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4F4664-6C2C-4C76-B585-4A3FD47CA8DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12885" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="src" sheetId="4" r:id="rId1"/>
@@ -22,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">src!$A$1:$BR$21</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -333,7 +332,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -793,11 +792,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -805,20 +801,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -828,6 +815,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -841,8 +834,14 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -853,8 +852,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -862,16 +861,16 @@
     <xf numFmtId="1" fontId="6" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный_src" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Обычный_Автотор" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Обычный_Лист1" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Обычный_Ручное распределение" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Обычный_src" xfId="3"/>
+    <cellStyle name="Обычный_Автотор" xfId="4"/>
+    <cellStyle name="Обычный_Лист1" xfId="1"/>
+    <cellStyle name="Обычный_Ручное распределение" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3516,7 +3515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5967,11 +5966,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF44"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView topLeftCell="X1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5986,51 +5985,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="AA1" s="66" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="AA1" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AH1" s="67" t="s">
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AH1" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -6097,10 +6096,10 @@
       <c r="AC4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AH4" s="65" t="s">
+      <c r="AH4" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="AI4" s="65"/>
+      <c r="AI4" s="67"/>
       <c r="AJ4" s="21"/>
       <c r="AK4" s="21"/>
       <c r="AL4" s="21"/>
@@ -6109,10 +6108,10 @@
       <c r="AO4" s="21"/>
       <c r="AP4" s="21"/>
       <c r="AQ4" s="21"/>
-      <c r="AR4" s="65" t="s">
+      <c r="AR4" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="AS4" s="65"/>
+      <c r="AS4" s="67"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
@@ -6210,91 +6209,91 @@
       <c r="A8" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64" t="s">
+      <c r="C8" s="68"/>
+      <c r="D8" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64" t="s">
+      <c r="E8" s="68"/>
+      <c r="F8" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64" t="s">
+      <c r="G8" s="68"/>
+      <c r="H8" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64" t="s">
+      <c r="I8" s="68"/>
+      <c r="J8" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="64"/>
+      <c r="K8" s="68"/>
       <c r="L8" s="26"/>
-      <c r="M8" s="64" t="s">
+      <c r="M8" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64" t="s">
+      <c r="N8" s="68"/>
+      <c r="O8" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64" t="s">
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="R8" s="64"/>
-      <c r="S8" s="64" t="s">
+      <c r="R8" s="68"/>
+      <c r="S8" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="T8" s="64"/>
-      <c r="U8" s="64" t="s">
+      <c r="T8" s="68"/>
+      <c r="U8" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="V8" s="64"/>
+      <c r="V8" s="68"/>
       <c r="AE8" s="16" t="s">
         <v>20</v>
       </c>
       <c r="AF8" s="15"/>
-      <c r="AH8" s="64" t="s">
+      <c r="AH8" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="AI8" s="64"/>
-      <c r="AJ8" s="64" t="s">
+      <c r="AI8" s="68"/>
+      <c r="AJ8" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="AK8" s="64"/>
-      <c r="AL8" s="64" t="s">
+      <c r="AK8" s="68"/>
+      <c r="AL8" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="AM8" s="64"/>
-      <c r="AN8" s="64" t="s">
+      <c r="AM8" s="68"/>
+      <c r="AN8" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="AO8" s="64"/>
-      <c r="AP8" s="64" t="s">
+      <c r="AO8" s="68"/>
+      <c r="AP8" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AQ8" s="64"/>
-      <c r="AR8" s="64" t="s">
+      <c r="AQ8" s="68"/>
+      <c r="AR8" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="AS8" s="64"/>
-      <c r="AT8" s="64" t="s">
+      <c r="AS8" s="68"/>
+      <c r="AT8" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="AU8" s="64"/>
-      <c r="AV8" s="64" t="s">
+      <c r="AU8" s="68"/>
+      <c r="AV8" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="AW8" s="64"/>
-      <c r="AX8" s="64" t="s">
+      <c r="AW8" s="68"/>
+      <c r="AX8" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="AY8" s="64"/>
-      <c r="AZ8" s="64" t="s">
+      <c r="AY8" s="68"/>
+      <c r="AZ8" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="BA8" s="64"/>
+      <c r="BA8" s="68"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
@@ -6424,10 +6423,10 @@
         <f>AND(AB44&lt;B44,AC44&gt;0)</f>
         <v>0</v>
       </c>
-      <c r="AH11" s="65" t="s">
+      <c r="AH11" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="AI11" s="65"/>
+      <c r="AI11" s="67"/>
       <c r="AJ11" s="21"/>
       <c r="AK11" s="21"/>
       <c r="AL11" s="21"/>
@@ -6436,10 +6435,10 @@
       <c r="AO11" s="21"/>
       <c r="AP11" s="21"/>
       <c r="AQ11" s="21"/>
-      <c r="AR11" s="65" t="s">
+      <c r="AR11" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="AS11" s="65"/>
+      <c r="AS11" s="67"/>
       <c r="AT11" s="21"/>
       <c r="AU11" s="21"/>
       <c r="AV11" s="21"/>
@@ -11079,21 +11078,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AH1:AU1"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
     <mergeCell ref="AV8:AW8"/>
     <mergeCell ref="AX8:AY8"/>
     <mergeCell ref="AZ8:BA8"/>
@@ -11106,6 +11090,21 @@
     <mergeCell ref="AP8:AQ8"/>
     <mergeCell ref="AR8:AS8"/>
     <mergeCell ref="AT8:AU8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AH1:AU1"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AR4:AS4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11113,11 +11112,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AS40" sqref="AS40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11131,206 +11130,206 @@
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="75"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="71"/>
       <c r="AK1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" s="73" t="s">
+      <c r="AL1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="AM1" s="74"/>
-      <c r="AN1" s="74"/>
-      <c r="AO1" s="74"/>
-      <c r="AP1" s="74"/>
-      <c r="AQ1" s="74"/>
-      <c r="AR1" s="74"/>
-      <c r="AS1" s="74"/>
-      <c r="AT1" s="74"/>
-      <c r="AU1" s="74"/>
-      <c r="AV1" s="74"/>
-      <c r="AW1" s="74"/>
-      <c r="AX1" s="74"/>
-      <c r="AY1" s="74"/>
-      <c r="AZ1" s="74"/>
-      <c r="BA1" s="74"/>
-      <c r="BB1" s="74"/>
-      <c r="BC1" s="74"/>
-      <c r="BD1" s="74"/>
-      <c r="BE1" s="75"/>
+      <c r="AM1" s="70"/>
+      <c r="AN1" s="70"/>
+      <c r="AO1" s="70"/>
+      <c r="AP1" s="70"/>
+      <c r="AQ1" s="70"/>
+      <c r="AR1" s="70"/>
+      <c r="AS1" s="70"/>
+      <c r="AT1" s="70"/>
+      <c r="AU1" s="70"/>
+      <c r="AV1" s="70"/>
+      <c r="AW1" s="70"/>
+      <c r="AX1" s="70"/>
+      <c r="AY1" s="70"/>
+      <c r="AZ1" s="70"/>
+      <c r="BA1" s="70"/>
+      <c r="BB1" s="70"/>
+      <c r="BC1" s="70"/>
+      <c r="BD1" s="70"/>
+      <c r="BE1" s="71"/>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="73" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="74"/>
-      <c r="U2" s="75"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="71"/>
       <c r="AK2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="AL2" s="73" t="s">
+      <c r="AL2" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="AM2" s="74"/>
-      <c r="AN2" s="74"/>
-      <c r="AO2" s="74"/>
-      <c r="AP2" s="74"/>
-      <c r="AQ2" s="74"/>
-      <c r="AR2" s="74"/>
-      <c r="AS2" s="74"/>
-      <c r="AT2" s="74"/>
-      <c r="AU2" s="75"/>
-      <c r="AV2" s="73" t="s">
+      <c r="AM2" s="70"/>
+      <c r="AN2" s="70"/>
+      <c r="AO2" s="70"/>
+      <c r="AP2" s="70"/>
+      <c r="AQ2" s="70"/>
+      <c r="AR2" s="70"/>
+      <c r="AS2" s="70"/>
+      <c r="AT2" s="70"/>
+      <c r="AU2" s="71"/>
+      <c r="AV2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="AW2" s="74"/>
-      <c r="AX2" s="74"/>
-      <c r="AY2" s="74"/>
-      <c r="AZ2" s="74"/>
-      <c r="BA2" s="74"/>
-      <c r="BB2" s="74"/>
-      <c r="BC2" s="74"/>
-      <c r="BD2" s="74"/>
-      <c r="BE2" s="75"/>
+      <c r="AW2" s="70"/>
+      <c r="AX2" s="70"/>
+      <c r="AY2" s="70"/>
+      <c r="AZ2" s="70"/>
+      <c r="BA2" s="70"/>
+      <c r="BB2" s="70"/>
+      <c r="BC2" s="70"/>
+      <c r="BD2" s="70"/>
+      <c r="BE2" s="71"/>
     </row>
     <row r="3" spans="1:57" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
-      <c r="U3" s="75"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="70"/>
+      <c r="T3" s="70"/>
+      <c r="U3" s="71"/>
       <c r="AK3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="AL3" s="73" t="s">
+      <c r="AL3" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AM3" s="74"/>
-      <c r="AN3" s="74"/>
-      <c r="AO3" s="74"/>
-      <c r="AP3" s="74"/>
-      <c r="AQ3" s="74"/>
-      <c r="AR3" s="74"/>
-      <c r="AS3" s="74"/>
-      <c r="AT3" s="74"/>
-      <c r="AU3" s="74"/>
-      <c r="AV3" s="74"/>
-      <c r="AW3" s="74"/>
-      <c r="AX3" s="74"/>
-      <c r="AY3" s="74"/>
-      <c r="AZ3" s="74"/>
-      <c r="BA3" s="74"/>
-      <c r="BB3" s="74"/>
-      <c r="BC3" s="74"/>
-      <c r="BD3" s="74"/>
-      <c r="BE3" s="75"/>
+      <c r="AM3" s="70"/>
+      <c r="AN3" s="70"/>
+      <c r="AO3" s="70"/>
+      <c r="AP3" s="70"/>
+      <c r="AQ3" s="70"/>
+      <c r="AR3" s="70"/>
+      <c r="AS3" s="70"/>
+      <c r="AT3" s="70"/>
+      <c r="AU3" s="70"/>
+      <c r="AV3" s="70"/>
+      <c r="AW3" s="70"/>
+      <c r="AX3" s="70"/>
+      <c r="AY3" s="70"/>
+      <c r="AZ3" s="70"/>
+      <c r="BA3" s="70"/>
+      <c r="BB3" s="70"/>
+      <c r="BC3" s="70"/>
+      <c r="BD3" s="70"/>
+      <c r="BE3" s="71"/>
     </row>
     <row r="4" spans="1:57" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="68" t="s">
+      <c r="C4" s="73"/>
+      <c r="D4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="68" t="s">
+      <c r="E4" s="73"/>
+      <c r="F4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="69"/>
-      <c r="H4" s="68" t="s">
+      <c r="G4" s="73"/>
+      <c r="H4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="69"/>
-      <c r="J4" s="68" t="s">
+      <c r="I4" s="73"/>
+      <c r="J4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="69"/>
-      <c r="L4" s="68" t="s">
+      <c r="K4" s="73"/>
+      <c r="L4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="69"/>
-      <c r="N4" s="68" t="s">
+      <c r="M4" s="73"/>
+      <c r="N4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="69"/>
-      <c r="P4" s="68" t="s">
+      <c r="O4" s="73"/>
+      <c r="P4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="68" t="s">
+      <c r="Q4" s="73"/>
+      <c r="R4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="69"/>
-      <c r="T4" s="68" t="s">
+      <c r="S4" s="73"/>
+      <c r="T4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="U4" s="69"/>
+      <c r="U4" s="73"/>
       <c r="W4" s="46" t="s">
         <v>31</v>
       </c>
@@ -11349,46 +11348,46 @@
       <c r="AK4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AL4" s="68" t="s">
+      <c r="AL4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="AM4" s="69"/>
-      <c r="AN4" s="68" t="s">
+      <c r="AM4" s="73"/>
+      <c r="AN4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="AO4" s="69"/>
-      <c r="AP4" s="68" t="s">
+      <c r="AO4" s="73"/>
+      <c r="AP4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="AQ4" s="69"/>
-      <c r="AR4" s="68" t="s">
+      <c r="AQ4" s="73"/>
+      <c r="AR4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="AS4" s="69"/>
-      <c r="AT4" s="68" t="s">
+      <c r="AS4" s="73"/>
+      <c r="AT4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="AU4" s="69"/>
-      <c r="AV4" s="68" t="s">
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="AW4" s="69"/>
-      <c r="AX4" s="68" t="s">
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="AY4" s="69"/>
-      <c r="AZ4" s="68" t="s">
+      <c r="AY4" s="73"/>
+      <c r="AZ4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="BA4" s="69"/>
-      <c r="BB4" s="68" t="s">
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="BC4" s="69"/>
-      <c r="BD4" s="68" t="s">
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="BE4" s="69"/>
+      <c r="BE4" s="73"/>
     </row>
     <row r="5" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
@@ -11543,117 +11542,117 @@
       <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="74">
         <v>1</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="76">
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="74">
         <v>2</v>
       </c>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="78"/>
-      <c r="AG6" s="79" t="s">
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="75"/>
+      <c r="S6" s="75"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="76"/>
+      <c r="AG6" s="77" t="s">
         <v>17</v>
       </c>
       <c r="AK6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="AL6" s="76">
+      <c r="AL6" s="74">
         <v>1</v>
       </c>
-      <c r="AM6" s="77"/>
-      <c r="AN6" s="77"/>
-      <c r="AO6" s="77"/>
-      <c r="AP6" s="77"/>
-      <c r="AQ6" s="77"/>
-      <c r="AR6" s="77"/>
-      <c r="AS6" s="77"/>
-      <c r="AT6" s="77"/>
-      <c r="AU6" s="78"/>
-      <c r="AV6" s="76">
+      <c r="AM6" s="75"/>
+      <c r="AN6" s="75"/>
+      <c r="AO6" s="75"/>
+      <c r="AP6" s="75"/>
+      <c r="AQ6" s="75"/>
+      <c r="AR6" s="75"/>
+      <c r="AS6" s="75"/>
+      <c r="AT6" s="75"/>
+      <c r="AU6" s="76"/>
+      <c r="AV6" s="74">
         <v>2</v>
       </c>
-      <c r="AW6" s="77"/>
-      <c r="AX6" s="77"/>
-      <c r="AY6" s="77"/>
-      <c r="AZ6" s="77"/>
-      <c r="BA6" s="77"/>
-      <c r="BB6" s="77"/>
-      <c r="BC6" s="77"/>
-      <c r="BD6" s="77"/>
-      <c r="BE6" s="78"/>
+      <c r="AW6" s="75"/>
+      <c r="AX6" s="75"/>
+      <c r="AY6" s="75"/>
+      <c r="AZ6" s="75"/>
+      <c r="BA6" s="75"/>
+      <c r="BB6" s="75"/>
+      <c r="BC6" s="75"/>
+      <c r="BD6" s="75"/>
+      <c r="BE6" s="76"/>
     </row>
     <row r="7" spans="1:57" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="74">
         <v>1</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="76">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="74">
         <v>2</v>
       </c>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
-      <c r="R7" s="77"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="77"/>
-      <c r="U7" s="78"/>
-      <c r="AG7" s="79"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="75"/>
+      <c r="T7" s="75"/>
+      <c r="U7" s="76"/>
+      <c r="AG7" s="77"/>
       <c r="AK7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AL7" s="76">
+      <c r="AL7" s="74">
         <v>1</v>
       </c>
-      <c r="AM7" s="77"/>
-      <c r="AN7" s="77"/>
-      <c r="AO7" s="77"/>
-      <c r="AP7" s="77"/>
-      <c r="AQ7" s="77"/>
-      <c r="AR7" s="77"/>
-      <c r="AS7" s="77"/>
-      <c r="AT7" s="77"/>
-      <c r="AU7" s="78"/>
-      <c r="AV7" s="76">
+      <c r="AM7" s="75"/>
+      <c r="AN7" s="75"/>
+      <c r="AO7" s="75"/>
+      <c r="AP7" s="75"/>
+      <c r="AQ7" s="75"/>
+      <c r="AR7" s="75"/>
+      <c r="AS7" s="75"/>
+      <c r="AT7" s="75"/>
+      <c r="AU7" s="76"/>
+      <c r="AV7" s="74">
         <v>2</v>
       </c>
-      <c r="AW7" s="77"/>
-      <c r="AX7" s="77"/>
-      <c r="AY7" s="77"/>
-      <c r="AZ7" s="77"/>
-      <c r="BA7" s="77"/>
-      <c r="BB7" s="77"/>
-      <c r="BC7" s="77"/>
-      <c r="BD7" s="77"/>
-      <c r="BE7" s="78"/>
+      <c r="AW7" s="75"/>
+      <c r="AX7" s="75"/>
+      <c r="AY7" s="75"/>
+      <c r="AZ7" s="75"/>
+      <c r="BA7" s="75"/>
+      <c r="BB7" s="75"/>
+      <c r="BC7" s="75"/>
+      <c r="BD7" s="75"/>
+      <c r="BE7" s="76"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
@@ -11955,11 +11954,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U10" s="41"/>
-      <c r="AC10" s="70" t="s">
+      <c r="AC10" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="AD10" s="71"/>
-      <c r="AE10" s="72"/>
+      <c r="AD10" s="79"/>
+      <c r="AE10" s="80"/>
       <c r="AK10" s="38" t="s">
         <v>10</v>
       </c>
@@ -12163,7 +12162,7 @@
       </c>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A12" s="87">
+      <c r="A12" s="64">
         <v>43497</v>
       </c>
       <c r="B12" s="44">
@@ -12345,7 +12344,7 @@
       </c>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A13" s="87">
+      <c r="A13" s="64">
         <v>43498</v>
       </c>
       <c r="B13" s="44">
@@ -12527,7 +12526,7 @@
       </c>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A14" s="87">
+      <c r="A14" s="64">
         <v>43499</v>
       </c>
       <c r="B14" s="44">
@@ -12709,7 +12708,7 @@
       </c>
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A15" s="87">
+      <c r="A15" s="64">
         <v>43500</v>
       </c>
       <c r="B15" s="45">
@@ -12891,7 +12890,7 @@
       </c>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A16" s="87">
+      <c r="A16" s="64">
         <v>43501</v>
       </c>
       <c r="B16" s="44">
@@ -13073,7 +13072,7 @@
       </c>
     </row>
     <row r="17" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A17" s="87">
+      <c r="A17" s="64">
         <v>43502</v>
       </c>
       <c r="B17" s="44">
@@ -13255,7 +13254,7 @@
       </c>
     </row>
     <row r="18" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A18" s="87">
+      <c r="A18" s="64">
         <v>43503</v>
       </c>
       <c r="B18" s="44">
@@ -13437,7 +13436,7 @@
       </c>
     </row>
     <row r="19" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A19" s="87">
+      <c r="A19" s="64">
         <v>43504</v>
       </c>
       <c r="B19" s="44">
@@ -13619,7 +13618,7 @@
       </c>
     </row>
     <row r="20" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A20" s="87">
+      <c r="A20" s="64">
         <v>43505</v>
       </c>
       <c r="B20" s="44">
@@ -13801,7 +13800,7 @@
       </c>
     </row>
     <row r="21" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A21" s="87">
+      <c r="A21" s="64">
         <v>43506</v>
       </c>
       <c r="B21" s="44">
@@ -13983,7 +13982,7 @@
       </c>
     </row>
     <row r="22" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A22" s="87">
+      <c r="A22" s="64">
         <v>43507</v>
       </c>
       <c r="B22" s="44">
@@ -14165,7 +14164,7 @@
       </c>
     </row>
     <row r="23" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A23" s="87">
+      <c r="A23" s="64">
         <v>43508</v>
       </c>
       <c r="B23" s="44">
@@ -14347,7 +14346,7 @@
       </c>
     </row>
     <row r="24" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A24" s="87">
+      <c r="A24" s="64">
         <v>43509</v>
       </c>
       <c r="B24" s="44">
@@ -14529,7 +14528,7 @@
       </c>
     </row>
     <row r="25" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A25" s="87">
+      <c r="A25" s="64">
         <v>43510</v>
       </c>
       <c r="B25" s="44">
@@ -14711,7 +14710,7 @@
       </c>
     </row>
     <row r="26" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A26" s="87">
+      <c r="A26" s="64">
         <v>43511</v>
       </c>
       <c r="B26" s="45">
@@ -14893,7 +14892,7 @@
       </c>
     </row>
     <row r="27" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A27" s="87">
+      <c r="A27" s="64">
         <v>43512</v>
       </c>
       <c r="B27" s="44">
@@ -15075,7 +15074,7 @@
       </c>
     </row>
     <row r="28" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A28" s="87">
+      <c r="A28" s="64">
         <v>43513</v>
       </c>
       <c r="B28" s="45">
@@ -15257,7 +15256,7 @@
       </c>
     </row>
     <row r="29" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A29" s="87">
+      <c r="A29" s="64">
         <v>43514</v>
       </c>
       <c r="B29" s="45">
@@ -15439,7 +15438,7 @@
       </c>
     </row>
     <row r="30" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A30" s="87">
+      <c r="A30" s="64">
         <v>43515</v>
       </c>
       <c r="B30" s="44">
@@ -15621,7 +15620,7 @@
       </c>
     </row>
     <row r="31" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A31" s="87">
+      <c r="A31" s="64">
         <v>43516</v>
       </c>
       <c r="B31" s="44">
@@ -15803,7 +15802,7 @@
       </c>
     </row>
     <row r="32" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A32" s="87">
+      <c r="A32" s="64">
         <v>43517</v>
       </c>
       <c r="B32" s="44">
@@ -15985,7 +15984,7 @@
       </c>
     </row>
     <row r="33" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A33" s="87">
+      <c r="A33" s="64">
         <v>43518</v>
       </c>
       <c r="B33" s="44">
@@ -16167,7 +16166,7 @@
       </c>
     </row>
     <row r="34" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A34" s="87">
+      <c r="A34" s="64">
         <v>43519</v>
       </c>
       <c r="B34" s="44">
@@ -16349,7 +16348,7 @@
       </c>
     </row>
     <row r="35" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A35" s="87">
+      <c r="A35" s="64">
         <v>43520</v>
       </c>
       <c r="B35" s="44">
@@ -16531,7 +16530,7 @@
       </c>
     </row>
     <row r="36" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A36" s="87">
+      <c r="A36" s="64">
         <v>43521</v>
       </c>
       <c r="B36" s="44">
@@ -16713,7 +16712,7 @@
       </c>
     </row>
     <row r="37" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A37" s="87">
+      <c r="A37" s="64">
         <v>43522</v>
       </c>
       <c r="B37" s="44">
@@ -16895,7 +16894,7 @@
       </c>
     </row>
     <row r="38" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A38" s="87">
+      <c r="A38" s="64">
         <v>43523</v>
       </c>
       <c r="B38" s="44">
@@ -17077,7 +17076,7 @@
       </c>
     </row>
     <row r="39" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A39" s="87">
+      <c r="A39" s="64">
         <v>43524</v>
       </c>
       <c r="B39" s="44">
@@ -17499,28 +17498,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B1:U1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="L2:U2"/>
-    <mergeCell ref="B3:U3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AT4:AU4"/>
-    <mergeCell ref="AV4:AW4"/>
-    <mergeCell ref="AX4:AY4"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="L6:U6"/>
-    <mergeCell ref="L7:U7"/>
-    <mergeCell ref="AG6:AG7"/>
     <mergeCell ref="AZ4:BA4"/>
     <mergeCell ref="BB4:BC4"/>
     <mergeCell ref="BD4:BE4"/>
@@ -17537,6 +17514,28 @@
     <mergeCell ref="AV6:BE6"/>
     <mergeCell ref="AL7:AU7"/>
     <mergeCell ref="AV7:BE7"/>
+    <mergeCell ref="AT4:AU4"/>
+    <mergeCell ref="AV4:AW4"/>
+    <mergeCell ref="AX4:AY4"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="L6:U6"/>
+    <mergeCell ref="L7:U7"/>
+    <mergeCell ref="AG6:AG7"/>
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="B3:U3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17545,10 +17544,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO40"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="BO25" sqref="BO25"/>
     </sheetView>
   </sheetViews>
@@ -17563,219 +17562,219 @@
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
-      <c r="AA1" s="74"/>
-      <c r="AB1" s="74"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="75"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="70"/>
+      <c r="AC1" s="70"/>
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="71"/>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="73" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="74"/>
-      <c r="X2" s="74"/>
-      <c r="Y2" s="74"/>
-      <c r="Z2" s="74"/>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
-      <c r="AC2" s="74"/>
-      <c r="AD2" s="74"/>
-      <c r="AE2" s="75"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="1:67" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="74"/>
-      <c r="X3" s="74"/>
-      <c r="Y3" s="74"/>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="74"/>
-      <c r="AB3" s="74"/>
-      <c r="AC3" s="74"/>
-      <c r="AD3" s="74"/>
-      <c r="AE3" s="75"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="70"/>
+      <c r="T3" s="70"/>
+      <c r="U3" s="70"/>
+      <c r="V3" s="70"/>
+      <c r="W3" s="70"/>
+      <c r="X3" s="70"/>
+      <c r="Y3" s="70"/>
+      <c r="Z3" s="70"/>
+      <c r="AA3" s="70"/>
+      <c r="AB3" s="70"/>
+      <c r="AC3" s="70"/>
+      <c r="AD3" s="70"/>
+      <c r="AE3" s="71"/>
     </row>
     <row r="4" spans="1:67" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="68" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="68" t="s">
+      <c r="F4" s="84"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="68" t="s">
+      <c r="I4" s="84"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="80"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="68" t="s">
+      <c r="L4" s="84"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="80"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="68" t="s">
+      <c r="O4" s="84"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="80"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="68" t="s">
+      <c r="R4" s="84"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="U4" s="80"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="68" t="s">
+      <c r="U4" s="84"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="68" t="s">
+      <c r="X4" s="84"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="69"/>
-      <c r="AC4" s="68" t="s">
+      <c r="AA4" s="84"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="AD4" s="80"/>
-      <c r="AE4" s="69"/>
-      <c r="AG4" s="68" t="s">
+      <c r="AD4" s="84"/>
+      <c r="AE4" s="73"/>
+      <c r="AG4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="68" t="s">
+      <c r="AH4" s="84"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="AK4" s="80"/>
-      <c r="AL4" s="69"/>
-      <c r="AM4" s="68" t="s">
+      <c r="AK4" s="84"/>
+      <c r="AL4" s="73"/>
+      <c r="AM4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="AN4" s="80"/>
-      <c r="AO4" s="69"/>
-      <c r="AP4" s="68" t="s">
+      <c r="AN4" s="84"/>
+      <c r="AO4" s="73"/>
+      <c r="AP4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="AQ4" s="80"/>
-      <c r="AR4" s="69"/>
-      <c r="AS4" s="68" t="s">
+      <c r="AQ4" s="84"/>
+      <c r="AR4" s="73"/>
+      <c r="AS4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="69"/>
-      <c r="BA4" s="68" t="s">
+      <c r="AT4" s="84"/>
+      <c r="AU4" s="73"/>
+      <c r="BA4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="BB4" s="80"/>
-      <c r="BC4" s="69"/>
-      <c r="BD4" s="68" t="s">
+      <c r="BB4" s="84"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="69"/>
-      <c r="BG4" s="68" t="s">
+      <c r="BE4" s="84"/>
+      <c r="BF4" s="73"/>
+      <c r="BG4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="69"/>
-      <c r="BJ4" s="68" t="s">
+      <c r="BH4" s="84"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="BK4" s="80"/>
-      <c r="BL4" s="69"/>
-      <c r="BM4" s="68" t="s">
+      <c r="BK4" s="84"/>
+      <c r="BL4" s="73"/>
+      <c r="BM4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="BN4" s="80"/>
-      <c r="BO4" s="69"/>
+      <c r="BN4" s="84"/>
+      <c r="BO4" s="73"/>
     </row>
     <row r="5" spans="1:67" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
@@ -17966,79 +17965,79 @@
       <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="74">
         <v>1</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="76">
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="74">
         <v>2</v>
       </c>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="77"/>
-      <c r="X6" s="77"/>
-      <c r="Y6" s="77"/>
-      <c r="Z6" s="77"/>
-      <c r="AA6" s="77"/>
-      <c r="AB6" s="77"/>
-      <c r="AC6" s="77"/>
-      <c r="AD6" s="77"/>
-      <c r="AE6" s="78"/>
+      <c r="R6" s="75"/>
+      <c r="S6" s="75"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="75"/>
+      <c r="W6" s="75"/>
+      <c r="X6" s="75"/>
+      <c r="Y6" s="75"/>
+      <c r="Z6" s="75"/>
+      <c r="AA6" s="75"/>
+      <c r="AB6" s="75"/>
+      <c r="AC6" s="75"/>
+      <c r="AD6" s="75"/>
+      <c r="AE6" s="76"/>
     </row>
     <row r="7" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="74">
         <v>1</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="76">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="74">
         <v>2</v>
       </c>
-      <c r="R7" s="77"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="77"/>
-      <c r="U7" s="77"/>
-      <c r="V7" s="77"/>
-      <c r="W7" s="77"/>
-      <c r="X7" s="77"/>
-      <c r="Y7" s="77"/>
-      <c r="Z7" s="77"/>
-      <c r="AA7" s="77"/>
-      <c r="AB7" s="77"/>
-      <c r="AC7" s="77"/>
-      <c r="AD7" s="77"/>
-      <c r="AE7" s="78"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="75"/>
+      <c r="T7" s="75"/>
+      <c r="U7" s="75"/>
+      <c r="V7" s="75"/>
+      <c r="W7" s="75"/>
+      <c r="X7" s="75"/>
+      <c r="Y7" s="75"/>
+      <c r="Z7" s="75"/>
+      <c r="AA7" s="75"/>
+      <c r="AB7" s="75"/>
+      <c r="AC7" s="75"/>
+      <c r="AD7" s="75"/>
+      <c r="AE7" s="76"/>
     </row>
     <row r="8" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
@@ -18326,11 +18325,11 @@
       <c r="AS10" s="82"/>
       <c r="AT10" s="82"/>
       <c r="AU10" s="83"/>
-      <c r="AW10" s="70" t="s">
+      <c r="AW10" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="AX10" s="71"/>
-      <c r="AY10" s="72"/>
+      <c r="AX10" s="79"/>
+      <c r="AY10" s="80"/>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
@@ -25358,24 +25357,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="AG10:AU10"/>
-    <mergeCell ref="BG4:BI4"/>
-    <mergeCell ref="BJ4:BL4"/>
-    <mergeCell ref="BM4:BO4"/>
-    <mergeCell ref="AW10:AY10"/>
-    <mergeCell ref="AS4:AU4"/>
-    <mergeCell ref="BD4:BF4"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="Q6:AE6"/>
-    <mergeCell ref="B7:P7"/>
-    <mergeCell ref="Q7:AE7"/>
-    <mergeCell ref="BA4:BC4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AM4:AO4"/>
-    <mergeCell ref="AJ4:AL4"/>
-    <mergeCell ref="AG4:AI4"/>
     <mergeCell ref="B1:AE1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="Q2:AE2"/>
@@ -25388,6 +25369,24 @@
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="Q6:AE6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="Q7:AE7"/>
+    <mergeCell ref="BA4:BC4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AM4:AO4"/>
+    <mergeCell ref="AJ4:AL4"/>
+    <mergeCell ref="AG4:AI4"/>
+    <mergeCell ref="AG10:AU10"/>
+    <mergeCell ref="BG4:BI4"/>
+    <mergeCell ref="BJ4:BL4"/>
+    <mergeCell ref="BM4:BO4"/>
+    <mergeCell ref="AW10:AY10"/>
+    <mergeCell ref="AS4:AU4"/>
+    <mergeCell ref="BD4:BF4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25396,11 +25395,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AC43" sqref="AC43:AF43"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -25416,109 +25415,109 @@
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="84"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="87"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="73" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="84"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="87"/>
     </row>
     <row r="3" spans="1:35" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="84"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="87"/>
     </row>
     <row r="4" spans="1:35" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="68" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="68" t="str">
+      <c r="F4" s="84"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="72" t="str">
         <f>B4</f>
         <v>г. Калининград, Магнитогорская ул., д.4</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="68" t="str">
+      <c r="I4" s="84"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="72" t="str">
         <f>E4</f>
         <v>г. Калининград, Большая Окружная 4-я ул., д.1 А, котельная</v>
       </c>
-      <c r="L4" s="80"/>
-      <c r="M4" s="69"/>
-      <c r="O4" s="68" t="str">
+      <c r="L4" s="84"/>
+      <c r="M4" s="73"/>
+      <c r="O4" s="72" t="str">
         <f>B4</f>
         <v>г. Калининград, Магнитогорская ул., д.4</v>
       </c>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="68" t="str">
+      <c r="P4" s="84"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="72" t="str">
         <f>E4</f>
         <v>г. Калининград, Большая Окружная 4-я ул., д.1 А, котельная</v>
       </c>
-      <c r="S4" s="80"/>
-      <c r="T4" s="69"/>
-      <c r="V4" s="68" t="str">
+      <c r="S4" s="84"/>
+      <c r="T4" s="73"/>
+      <c r="V4" s="72" t="str">
         <f>B4</f>
         <v>г. Калининград, Магнитогорская ул., д.4</v>
       </c>
-      <c r="W4" s="80"/>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="68" t="str">
+      <c r="W4" s="84"/>
+      <c r="X4" s="73"/>
+      <c r="Y4" s="72" t="str">
         <f>E4</f>
         <v>г. Калининград, Большая Окружная 4-я ул., д.1 А, котельная</v>
       </c>
-      <c r="Z4" s="80"/>
-      <c r="AA4" s="69"/>
+      <c r="Z4" s="84"/>
+      <c r="AA4" s="73"/>
       <c r="AC4" s="62" t="str">
         <f>V4</f>
         <v>г. Калининград, Магнитогорская ул., д.4</v>
@@ -25635,42 +25634,42 @@
       <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="74">
         <v>4</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="76">
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="74">
         <v>3</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
       <c r="M6" s="86"/>
     </row>
     <row r="7" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="74">
         <v>3</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="76">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="74">
         <v>4</v>
       </c>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="77"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
       <c r="M7" s="86"/>
       <c r="AD7" s="85" t="s">
         <v>25</v>
@@ -29697,17 +29696,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="O10:T10"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H7:M7"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:M2"/>
@@ -29715,6 +29703,17 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="H4:J4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="O10:T10"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>